<commit_message>
Updated time long (wrong directory)
</commit_message>
<xml_diff>
--- a/docs/time_logs/Stephen_time_log.xlsx
+++ b/docs/time_logs/Stephen_time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\Senior Project 1\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8E95FD-5055-4CDD-925F-DC0CEF409E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC85A173-DECC-4BD8-99FC-7818966D83D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2712" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Start Time</t>
   </si>
@@ -81,7 +81,13 @@
     <t>Worked on background.tex and business_context.tex</t>
   </si>
   <si>
-    <t>10/25/2021 05:24 P.M.</t>
+    <t>10/27/2021 1:00 P.M.</t>
+  </si>
+  <si>
+    <t>10/27/2021 2:00 P.M.</t>
+  </si>
+  <si>
+    <t>Created gantt chart and made additional small changes to scope</t>
   </si>
 </sst>
 </file>
@@ -133,10 +139,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +460,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -467,12 +473,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -541,8 +547,8 @@
       <c r="C6" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D6" s="9">
-        <v>0.16666666666666666</v>
+      <c r="D6" s="8">
+        <v>0.17361111111111113</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -552,9 +558,18 @@
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>

</xml_diff>

<commit_message>
time log (should have been pushed sooner)
</commit_message>
<xml_diff>
--- a/docs/time_logs/Stephen_time_log.xlsx
+++ b/docs/time_logs/Stephen_time_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\Senior Project 1\netbsd-wifi-browser\docs\time_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\Senior Project 2\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0AAB8E-C983-41D3-BFA9-591BB615C974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE94F1D2-0D07-4614-93F1-33059145EE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Start Time</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t xml:space="preserve">Finished writing description and external interfaces </t>
+  </si>
+  <si>
+    <t>01/12/2021 3:00 P.M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Spent </t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -659,10 +665,17 @@
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
+      <c r="C14" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added makefile, fixed a few things
</commit_message>
<xml_diff>
--- a/docs/time_logs/Stephen_time_log.xlsx
+++ b/docs/time_logs/Stephen_time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\Senior Project 2\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC20291F-9E48-49CD-BB77-CA62C4F17C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68C3C89-9E5A-451A-8F05-BC03A303FC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Start Time</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>01/12/2021 3:00 P.M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up NetBSD on VM, wrote a makefile. Makefile had to be specific, took too much time. (I will probably work over 40 hours this quarter, but I will document all time spent). </t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -668,6 +671,12 @@
       <c r="C13" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="D13" s="8">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>

</xml_diff>

<commit_message>
stephen: keep forgetting to clock in (clock out)
</commit_message>
<xml_diff>
--- a/docs/time_logs/Stephen_time_log.xlsx
+++ b/docs/time_logs/Stephen_time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\Senior Project 2\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544BEAB1-A15F-43AE-93CF-9481AFF1398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6183CB-02E0-421B-AE0C-D48D9610CFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Start Time</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fixed a few things, did some error checking. Ready to start processing commands from API.  </t>
+  </si>
+  <si>
+    <t>01/24/2021 1:00 P.M.</t>
+  </si>
+  <si>
+    <t>1/24/2021 11:00 A.M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Made it more secure. Can't break the cli, ready for API implementation. </t>
   </si>
 </sst>
 </file>
@@ -539,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -815,6 +824,23 @@
         <v>44</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
stephen: clock in (ignore last clockout will finish 4hrs)
</commit_message>
<xml_diff>
--- a/docs/time_logs/Stephen_time_log.xlsx
+++ b/docs/time_logs/Stephen_time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\Senior Project 3\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EF3E59-BEED-4C85-BD0D-91EB3E8476A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706401B1-FBD8-44A1-8805-920A3AF74C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -662,7 +662,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1156,10 +1156,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>